<commit_message>
fix:bug fixed in uploading merged file and add:added download merged file
</commit_message>
<xml_diff>
--- a/kpi.xlsx
+++ b/kpi.xlsx
@@ -375,30 +375,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Name</v>
+        <v>rno</v>
       </c>
       <c r="B1" t="str">
-        <v>Email</v>
+        <v>fname</v>
+      </c>
+      <c r="C1" t="str">
+        <v>lname</v>
+      </c>
+      <c r="D1" t="str">
+        <v>size</v>
+      </c>
+      <c r="E1" t="str">
+        <v>block</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>Arjun</v>
+      <c r="A2">
+        <v>323</v>
       </c>
       <c r="B2" t="str">
-        <v>arjun@qac.in</v>
+        <v>testa</v>
+      </c>
+      <c r="C2" t="str">
+        <v>popp</v>
+      </c>
+      <c r="D2" t="str">
+        <v>c</v>
+      </c>
+      <c r="E2" t="str">
+        <v>g2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>87987</v>
+      </c>
+      <c r="B3" t="str">
+        <v>ksk</v>
+      </c>
+      <c r="C3" t="str">
+        <v>akka</v>
+      </c>
+      <c r="D3" t="str">
+        <v>a</v>
+      </c>
+      <c r="E3" t="str">
+        <v>g3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>233</v>
+      </c>
+      <c r="B4" t="str">
+        <v>qe</v>
+      </c>
+      <c r="C4" t="str">
+        <v>eer</v>
+      </c>
+      <c r="D4" t="str">
+        <v>b</v>
+      </c>
+      <c r="E4" t="str">
+        <v>g3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>565</v>
+      </c>
+      <c r="B5" t="str">
+        <v>vdgd</v>
+      </c>
+      <c r="C5" t="str">
+        <v>ffsd</v>
+      </c>
+      <c r="D5" t="str">
+        <v>a</v>
+      </c>
+      <c r="E5" t="str">
+        <v>g3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>567</v>
+      </c>
+      <c r="B6" t="str">
+        <v>dfg</v>
+      </c>
+      <c r="C6" t="str">
+        <v>rer</v>
+      </c>
+      <c r="D6" t="str">
+        <v>c</v>
+      </c>
+      <c r="E6" t="str">
+        <v>g2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>232</v>
+      </c>
+      <c r="B7" t="str">
+        <v>gjg</v>
+      </c>
+      <c r="C7" t="str">
+        <v>poi</v>
+      </c>
+      <c r="D7" t="str">
+        <v>b</v>
+      </c>
+      <c r="E7" t="str">
+        <v>g2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>